<commit_message>
Update Casos confirmados 13-04-2020.xlsx
</commit_message>
<xml_diff>
--- a/Casos confirmados 13-04-2020.xlsx
+++ b/Casos confirmados 13-04-2020.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kyro\Documents\GitHub\Covid-19-Colombia\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{CD9F20AB-1A17-4825-95A4-6C6B35C695F8}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70C5B51F-9566-4B5D-BCC6-3927E68F739B}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Casos confirmados" sheetId="1" r:id="rId1"/>
@@ -1914,11 +1914,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <sheetPr filterMode="1"/>
   <dimension ref="A1:N2853"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2812" workbookViewId="0">
-      <selection activeCell="O2817" sqref="O2817"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J8" sqref="J8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7051,7 +7050,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="153" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A153">
         <v>152</v>
       </c>
@@ -7090,7 +7089,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="154" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A154">
         <v>153</v>
       </c>
@@ -7228,7 +7227,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="158" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A158">
         <v>157</v>
       </c>
@@ -8257,7 +8256,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="189" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A189">
         <v>188</v>
       </c>
@@ -8560,7 +8559,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="198" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A198">
         <v>197</v>
       </c>
@@ -9721,7 +9720,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="233" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="233" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A233">
         <v>232</v>
       </c>
@@ -10321,7 +10320,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="251" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="251" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A251">
         <v>250</v>
       </c>
@@ -10690,7 +10689,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="262" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="262" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A262">
         <v>261</v>
       </c>
@@ -11521,7 +11520,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="287" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="287" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A287">
         <v>286</v>
       </c>
@@ -12451,7 +12450,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="315" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="315" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A315">
         <v>314</v>
       </c>
@@ -12853,7 +12852,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="327" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="327" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A327">
         <v>326</v>
       </c>
@@ -14940,7 +14939,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="390" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="390" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A390">
         <v>389</v>
       </c>
@@ -16134,7 +16133,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="426" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="426" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A426">
         <v>425</v>
       </c>
@@ -18319,7 +18318,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="492" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="492" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A492">
         <v>491</v>
       </c>
@@ -18952,7 +18951,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="511" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="511" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A511">
         <v>510</v>
       </c>
@@ -19090,7 +19089,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="515" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="515" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A515">
         <v>514</v>
       </c>
@@ -19723,7 +19722,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="534" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="534" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A534">
         <v>533</v>
       </c>
@@ -19795,7 +19794,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="536" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="536" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A536">
         <v>535</v>
       </c>
@@ -20065,7 +20064,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="544" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="544" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A544">
         <v>543</v>
       </c>
@@ -20830,7 +20829,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="567" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="567" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A567">
         <v>566</v>
       </c>
@@ -20935,7 +20934,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="570" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="570" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A570">
         <v>569</v>
       </c>
@@ -21535,7 +21534,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="588" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="588" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A588">
         <v>587</v>
       </c>
@@ -22597,7 +22596,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="620" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="620" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A620">
         <v>619</v>
       </c>
@@ -24418,7 +24417,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="675" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="675" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A675">
         <v>674</v>
       </c>
@@ -25513,7 +25512,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="708" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="708" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A708">
         <v>707</v>
       </c>
@@ -25618,7 +25617,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="711" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="711" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A711">
         <v>710</v>
       </c>
@@ -25756,7 +25755,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="715" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="715" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A715">
         <v>714</v>
       </c>
@@ -26026,7 +26025,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="723" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="723" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A723">
         <v>722</v>
       </c>
@@ -27649,7 +27648,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="772" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="772" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A772">
         <v>771</v>
       </c>
@@ -27919,7 +27918,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="780" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="780" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A780">
         <v>779</v>
       </c>
@@ -29542,7 +29541,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="829" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="829" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A829">
         <v>828</v>
       </c>
@@ -30076,7 +30075,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="845" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="845" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A845">
         <v>844</v>
       </c>
@@ -30742,7 +30741,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="865" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="865" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A865">
         <v>864</v>
       </c>
@@ -31606,7 +31605,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="891" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="891" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A891">
         <v>890</v>
       </c>
@@ -32701,7 +32700,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="924" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="924" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A924">
         <v>923</v>
       </c>
@@ -34820,7 +34819,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="988" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="988" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A988">
         <v>987</v>
       </c>
@@ -34859,7 +34858,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="989" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="989" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A989">
         <v>988</v>
       </c>
@@ -34931,7 +34930,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="991" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="991" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A991">
         <v>990</v>
       </c>
@@ -36622,7 +36621,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="1042" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="1042" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1042">
         <v>1041</v>
       </c>
@@ -37189,7 +37188,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="1059" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="1059" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1059">
         <v>1058</v>
       </c>
@@ -37393,7 +37392,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="1065" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="1065" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1065">
         <v>1064</v>
       </c>
@@ -37861,7 +37860,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="1079" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="1079" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1079">
         <v>1078</v>
       </c>
@@ -38461,7 +38460,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="1097" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="1097" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1097">
         <v>1096</v>
       </c>
@@ -39655,7 +39654,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="1133" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="1133" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1133">
         <v>1132</v>
       </c>
@@ -40915,7 +40914,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="1171" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="1171" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1171">
         <v>1170</v>
       </c>
@@ -41911,7 +41910,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="1201" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="1201" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1201">
         <v>1200</v>
       </c>
@@ -42016,7 +42015,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="1204" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="1204" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1204">
         <v>1203</v>
       </c>
@@ -42649,7 +42648,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="1223" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="1223" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1223">
         <v>1222</v>
       </c>
@@ -42853,7 +42852,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="1229" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="1229" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1229">
         <v>1228</v>
       </c>
@@ -43189,7 +43188,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="1239" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="1239" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1239">
         <v>1238</v>
       </c>
@@ -43426,7 +43425,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="1246" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="1246" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1246">
         <v>1245</v>
       </c>
@@ -44554,7 +44553,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="1280" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="1280" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1280">
         <v>1279</v>
       </c>
@@ -45220,7 +45219,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="1300" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="1300" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1300">
         <v>1299</v>
       </c>
@@ -45259,7 +45258,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="1301" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="1301" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1301">
         <v>1300</v>
       </c>
@@ -45463,7 +45462,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="1307" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="1307" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1307">
         <v>1306</v>
       </c>
@@ -46756,7 +46755,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="1346" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="1346" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1346">
         <v>1345</v>
       </c>
@@ -47653,7 +47652,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="1373" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="1373" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1373">
         <v>1372</v>
       </c>
@@ -48121,7 +48120,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="1387" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="1387" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1387">
         <v>1386</v>
       </c>
@@ -48226,7 +48225,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="1390" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="1390" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1390">
         <v>1389</v>
       </c>
@@ -49321,7 +49320,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="1423" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="1423" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1423">
         <v>1422</v>
       </c>
@@ -50449,7 +50448,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="1457" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="1457" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1457">
         <v>1456</v>
       </c>
@@ -51445,7 +51444,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="1487" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="1487" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1487">
         <v>1486</v>
       </c>
@@ -52078,7 +52077,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="1506" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="1506" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1506">
         <v>1505</v>
       </c>
@@ -52381,7 +52380,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="1515" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="1515" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1515">
         <v>1514</v>
       </c>
@@ -53212,7 +53211,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="1540" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="1540" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1540">
         <v>1539</v>
       </c>
@@ -54373,7 +54372,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="1575" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="1575" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1575">
         <v>1574</v>
       </c>
@@ -54643,7 +54642,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="1583" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="1583" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1583">
         <v>1582</v>
       </c>
@@ -54682,7 +54681,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="1584" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="1584" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1584">
         <v>1583</v>
       </c>
@@ -55249,7 +55248,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="1601" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="1601" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1601">
         <v>1600</v>
       </c>
@@ -56179,7 +56178,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="1629" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="1629" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1629">
         <v>1628</v>
       </c>
@@ -57802,7 +57801,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="1678" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="1678" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1678">
         <v>1677</v>
       </c>
@@ -59491,7 +59490,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="1729" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="1729" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1729">
         <v>1728</v>
       </c>
@@ -60487,7 +60486,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="1759" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="1759" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1759">
         <v>1758</v>
       </c>
@@ -62209,7 +62208,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="1811" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="1811" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1811">
         <v>1810</v>
       </c>
@@ -62545,7 +62544,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="1821" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="1821" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1821">
         <v>1820</v>
       </c>
@@ -63508,7 +63507,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="1850" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="1850" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1850">
         <v>1849</v>
       </c>
@@ -64471,7 +64470,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="1879" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="1879" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1879">
         <v>1878</v>
       </c>
@@ -65698,7 +65697,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="1916" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="1916" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1916">
         <v>1915</v>
       </c>
@@ -65803,7 +65802,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="1919" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="1919" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1919">
         <v>1918</v>
       </c>
@@ -66139,7 +66138,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="1929" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="1929" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1929">
         <v>1928</v>
       </c>
@@ -66178,7 +66177,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="1930" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="1930" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1930">
         <v>1929</v>
       </c>
@@ -67603,7 +67602,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="1973" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="1973" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1973">
         <v>1972</v>
       </c>
@@ -68500,7 +68499,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="2000" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="2000" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2000">
         <v>1999</v>
       </c>
@@ -69331,7 +69330,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="2025" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="2025" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2025">
         <v>2024</v>
       </c>
@@ -69865,7 +69864,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2041" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="2041" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2041">
         <v>2040</v>
       </c>
@@ -70597,7 +70596,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="2063" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="2063" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2063">
         <v>2062</v>
       </c>
@@ -70801,7 +70800,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="2069" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="2069" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2069">
         <v>2068</v>
       </c>
@@ -70972,7 +70971,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="2074" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="2074" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2074">
         <v>2073</v>
       </c>
@@ -71935,7 +71934,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="2103" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="2103" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2103">
         <v>2102</v>
       </c>
@@ -72172,7 +72171,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="2110" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="2110" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2110">
         <v>2109</v>
       </c>
@@ -72574,7 +72573,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="2122" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="2122" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2122">
         <v>2121</v>
       </c>
@@ -72811,7 +72810,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="2129" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="2129" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2129">
         <v>2128</v>
       </c>
@@ -72883,7 +72882,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="2131" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="2131" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2131">
         <v>2130</v>
       </c>
@@ -74044,7 +74043,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="2166" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="2166" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2166">
         <v>2165</v>
       </c>
@@ -74281,7 +74280,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="2173" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="2173" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2173">
         <v>2172</v>
       </c>
@@ -74779,7 +74778,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="2188" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="2188" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2188">
         <v>2187</v>
       </c>
@@ -77491,7 +77490,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="2270" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="2270" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2270">
         <v>2269</v>
       </c>
@@ -77827,7 +77826,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="2280" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="2280" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2280">
         <v>2279</v>
       </c>
@@ -81133,7 +81132,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="2380" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="2380" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2380">
         <v>2379</v>
       </c>
@@ -81172,7 +81171,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="2381" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="2381" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2381">
         <v>2380</v>
       </c>
@@ -81574,7 +81573,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="2393" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="2393" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2393">
         <v>2392</v>
       </c>
@@ -81811,7 +81810,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="2400" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="2400" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2400">
         <v>2399</v>
       </c>
@@ -85645,7 +85644,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="2516" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="2516" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2516">
         <v>2515</v>
       </c>
@@ -85816,7 +85815,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="2521" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="2521" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2521">
         <v>2520</v>
       </c>
@@ -88330,7 +88329,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="2597" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="2597" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2597">
         <v>2596</v>
       </c>
@@ -88930,7 +88929,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="2615" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="2615" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2615">
         <v>2614</v>
       </c>
@@ -89398,7 +89397,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="2629" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="2629" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2629">
         <v>2628</v>
       </c>
@@ -89536,7 +89535,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="2633" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="2633" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2633">
         <v>2632</v>
       </c>
@@ -89839,7 +89838,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="2642" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="2642" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2642">
         <v>2641</v>
       </c>
@@ -90076,7 +90075,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="2649" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="2649" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2649">
         <v>2648</v>
       </c>
@@ -92755,7 +92754,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="2730" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="2730" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2730">
         <v>2729</v>
       </c>
@@ -95269,7 +95268,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="2806" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="2806" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2806">
         <v>2805</v>
       </c>
@@ -96860,11 +96859,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:L2853" xr:uid="{00000000-0009-0000-0000-000000000000}">
-    <filterColumn colId="9">
-      <filters blank="1"/>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A1:L2853" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
     <ignoredError sqref="F2 F3:F1407 F1408:F1486 F1487:F1580 F1581:F1781 F1782:F2055 F2056:F2224 F2225:F2474 F2475:F2710 F2711:F2777 F2778:F2854" twoDigitTextYear="1"/>

</xml_diff>